<commit_message>
pushing batch status file for sentiment analysis using llm models
</commit_message>
<xml_diff>
--- a/Projects/SentimentAnalysis/Data/Process/batch_status.xlsx
+++ b/Projects/SentimentAnalysis/Data/Process/batch_status.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -519,6 +519,86 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>200</v>
+      </c>
+      <c r="B6" t="n">
+        <v>250</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>250</v>
+      </c>
+      <c r="B7" t="n">
+        <v>300</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>300</v>
+      </c>
+      <c r="B8" t="n">
+        <v>350</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>350</v>
+      </c>
+      <c r="B9" t="n">
+        <v>400</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.9399999999999999</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>400</v>
+      </c>
+      <c r="B10" t="n">
+        <v>450</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>processed</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>